<commit_message>
Zeitplan wurde für IPA modifiziert
</commit_message>
<xml_diff>
--- a/Doku/zeitplanIPA.xlsx
+++ b/Doku/zeitplanIPA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProbeIPA\Doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ProbeIPA\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DB8A97D3-EB08-488D-A51E-D6CC054DB3CA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA871CF1-EEFF-4044-A81E-660DBB86CC53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
   <si>
     <t>Zustand</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Schlusswort verfassen</t>
+  </si>
+  <si>
+    <t>snip</t>
   </si>
 </sst>
 </file>
@@ -1270,6 +1273,57 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="22" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="22" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="22" xfId="22" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="20" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" xfId="21" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1279,18 +1333,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="22" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1307,72 +1349,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="22" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" xfId="21" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="22" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="22" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="22" xfId="22" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="20" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" xfId="19" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="40 % - Akzent6" xfId="22" builtinId="51"/>
+    <cellStyle name="40% - Accent6" xfId="22" builtinId="51"/>
+    <cellStyle name="Accent2" xfId="19" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="20" builtinId="37"/>
+    <cellStyle name="Accent5" xfId="21" builtinId="45"/>
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Akzent2" xfId="19" builtinId="33"/>
-    <cellStyle name="Akzent3" xfId="20" builtinId="37"/>
-    <cellStyle name="Akzent5" xfId="21" builtinId="45"/>
-    <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Überschrift" xfId="8" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2007,13 +2010,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642E310D-AE39-45A6-96C4-D01CF450F527}">
-  <dimension ref="B2:U57"/>
+  <dimension ref="B2:Y57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.75" customWidth="1"/>
     <col min="3" max="3" width="3.375" customWidth="1"/>
@@ -2023,68 +2026,68 @@
   <sheetData>
     <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="91" t="s">
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="92"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="91" t="s">
+      <c r="G3" s="105"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="92"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="91" t="s">
+      <c r="J3" s="105"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="92"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="91" t="s">
+      <c r="M3" s="105"/>
+      <c r="N3" s="106"/>
+      <c r="O3" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="91" t="s">
+      <c r="P3" s="105"/>
+      <c r="Q3" s="106"/>
+      <c r="R3" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="92"/>
-      <c r="T3" s="93"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="106"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="94"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="94" t="s">
+      <c r="B4" s="107"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="95"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="94" t="s">
+      <c r="G4" s="108"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="95"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="94" t="s">
+      <c r="J4" s="108"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="95"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="94" t="s">
+      <c r="M4" s="108"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="94" t="s">
+      <c r="P4" s="108"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="95"/>
-      <c r="T4" s="96"/>
+      <c r="S4" s="108"/>
+      <c r="T4" s="109"/>
     </row>
     <row r="5" spans="2:20" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
@@ -2146,34 +2149,34 @@
       </c>
     </row>
     <row r="6" spans="2:20" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="104"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="105"/>
-      <c r="P6" s="105"/>
-      <c r="Q6" s="105"/>
-      <c r="R6" s="105"/>
-      <c r="S6" s="105"/>
-      <c r="T6" s="106"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="86"/>
     </row>
     <row r="7" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="87">
+      <c r="C7" s="90">
         <v>1</v>
       </c>
-      <c r="D7" s="89" t="s">
+      <c r="D7" s="94" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -2196,9 +2199,9 @@
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="85"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="99"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="98"/>
       <c r="E8" s="32" t="s">
         <v>1</v>
       </c>
@@ -2219,11 +2222,11 @@
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="85"/>
-      <c r="C9" s="87">
+      <c r="B9" s="102"/>
+      <c r="C9" s="90">
         <v>2</v>
       </c>
-      <c r="D9" s="89" t="s">
+      <c r="D9" s="94" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -2246,9 +2249,9 @@
       <c r="T9" s="5"/>
     </row>
     <row r="10" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="85"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="90"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="95"/>
       <c r="E10" s="10" t="s">
         <v>1</v>
       </c>
@@ -2269,11 +2272,11 @@
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="85"/>
-      <c r="C11" s="87">
+      <c r="B11" s="102"/>
+      <c r="C11" s="90">
         <v>3</v>
       </c>
-      <c r="D11" s="89" t="s">
+      <c r="D11" s="94" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -2296,9 +2299,9 @@
       <c r="T11" s="53"/>
     </row>
     <row r="12" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="85"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="90"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="95"/>
       <c r="E12" s="10" t="s">
         <v>1</v>
       </c>
@@ -2319,11 +2322,11 @@
       <c r="T12" s="63"/>
     </row>
     <row r="13" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="85"/>
-      <c r="C13" s="87">
+      <c r="B13" s="102"/>
+      <c r="C13" s="90">
         <v>4</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="94" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -2346,9 +2349,9 @@
       <c r="T13" s="5"/>
     </row>
     <row r="14" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="86"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="90"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="95"/>
       <c r="E14" s="10" t="s">
         <v>1</v>
       </c>
@@ -2369,13 +2372,13 @@
       <c r="T14" s="10"/>
     </row>
     <row r="15" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="87">
+      <c r="C15" s="90">
         <v>5</v>
       </c>
-      <c r="D15" s="103" t="s">
+      <c r="D15" s="92" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -2398,9 +2401,9 @@
       <c r="T15" s="5"/>
     </row>
     <row r="16" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="85"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="100"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="93"/>
       <c r="E16" s="10" t="s">
         <v>1</v>
       </c>
@@ -2420,12 +2423,12 @@
       <c r="S16" s="9"/>
       <c r="T16" s="10"/>
     </row>
-    <row r="17" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="85"/>
-      <c r="C17" s="87">
+    <row r="17" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="102"/>
+      <c r="C17" s="90">
         <v>6</v>
       </c>
-      <c r="D17" s="89" t="s">
+      <c r="D17" s="94" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -2446,11 +2449,14 @@
       <c r="R17" s="51"/>
       <c r="S17" s="40"/>
       <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="85"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="100"/>
+      <c r="Y17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="102"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="93"/>
       <c r="E18" s="10" t="s">
         <v>1</v>
       </c>
@@ -2470,12 +2476,12 @@
       <c r="S18" s="9"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="85"/>
-      <c r="C19" s="87">
+    <row r="19" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="102"/>
+      <c r="C19" s="90">
         <v>7</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="92" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2497,10 +2503,10 @@
       <c r="S19" s="40"/>
       <c r="T19" s="5"/>
     </row>
-    <row r="20" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="85"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="100"/>
+    <row r="20" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="102"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="93"/>
       <c r="E20" s="10" t="s">
         <v>1</v>
       </c>
@@ -2520,12 +2526,12 @@
       <c r="S20" s="9"/>
       <c r="T20" s="10"/>
     </row>
-    <row r="21" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="85"/>
-      <c r="C21" s="87">
+    <row r="21" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="102"/>
+      <c r="C21" s="90">
         <v>8</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="94" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -2547,10 +2553,10 @@
       <c r="S21" s="40"/>
       <c r="T21" s="5"/>
     </row>
-    <row r="22" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="85"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="90"/>
+    <row r="22" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="102"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="95"/>
       <c r="E22" s="10" t="s">
         <v>1</v>
       </c>
@@ -2570,12 +2576,12 @@
       <c r="S22" s="9"/>
       <c r="T22" s="10"/>
     </row>
-    <row r="23" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="85"/>
-      <c r="C23" s="87">
+    <row r="23" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="102"/>
+      <c r="C23" s="90">
         <v>9</v>
       </c>
-      <c r="D23" s="89" t="s">
+      <c r="D23" s="94" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -2597,10 +2603,10 @@
       <c r="S23" s="40"/>
       <c r="T23" s="5"/>
     </row>
-    <row r="24" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="86"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="90"/>
+    <row r="24" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="103"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="95"/>
       <c r="E24" s="10" t="s">
         <v>1</v>
       </c>
@@ -2620,14 +2626,14 @@
       <c r="S24" s="57"/>
       <c r="T24" s="32"/>
     </row>
-    <row r="25" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="101" t="s">
+    <row r="25" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="87">
+      <c r="C25" s="90">
         <v>10</v>
       </c>
-      <c r="D25" s="89" t="s">
+      <c r="D25" s="94" t="s">
         <v>41</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -2649,10 +2655,10 @@
       <c r="S25" s="40"/>
       <c r="T25" s="5"/>
     </row>
-    <row r="26" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="102"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="90"/>
+    <row r="26" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="100"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="95"/>
       <c r="E26" s="10" t="s">
         <v>1</v>
       </c>
@@ -2672,14 +2678,14 @@
       <c r="S26" s="9"/>
       <c r="T26" s="10"/>
     </row>
-    <row r="27" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="84" t="s">
+    <row r="27" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="87">
+      <c r="C27" s="90">
         <v>11</v>
       </c>
-      <c r="D27" s="89" t="s">
+      <c r="D27" s="94" t="s">
         <v>39</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -2701,10 +2707,10 @@
       <c r="S27" s="40"/>
       <c r="T27" s="5"/>
     </row>
-    <row r="28" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="85"/>
-      <c r="C28" s="88"/>
-      <c r="D28" s="90"/>
+    <row r="28" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="102"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="95"/>
       <c r="E28" s="10" t="s">
         <v>1</v>
       </c>
@@ -2724,12 +2730,12 @@
       <c r="S28" s="9"/>
       <c r="T28" s="10"/>
     </row>
-    <row r="29" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="85"/>
-      <c r="C29" s="87">
+    <row r="29" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="102"/>
+      <c r="C29" s="90">
         <v>12</v>
       </c>
-      <c r="D29" s="89" t="s">
+      <c r="D29" s="94" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -2751,10 +2757,10 @@
       <c r="S29" s="40"/>
       <c r="T29" s="5"/>
     </row>
-    <row r="30" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="85"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="90"/>
+    <row r="30" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="102"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="95"/>
       <c r="E30" s="10" t="s">
         <v>1</v>
       </c>
@@ -2774,12 +2780,12 @@
       <c r="S30" s="9"/>
       <c r="T30" s="10"/>
     </row>
-    <row r="31" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="85"/>
-      <c r="C31" s="87">
+    <row r="31" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="102"/>
+      <c r="C31" s="90">
         <v>13</v>
       </c>
-      <c r="D31" s="89" t="s">
+      <c r="D31" s="94" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -2801,10 +2807,10 @@
       <c r="S31" s="40"/>
       <c r="T31" s="5"/>
     </row>
-    <row r="32" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="85"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="90"/>
+    <row r="32" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="102"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="95"/>
       <c r="E32" s="10" t="s">
         <v>1</v>
       </c>
@@ -2825,11 +2831,11 @@
       <c r="T32" s="10"/>
     </row>
     <row r="33" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="85"/>
-      <c r="C33" s="87">
+      <c r="B33" s="102"/>
+      <c r="C33" s="90">
         <v>14</v>
       </c>
-      <c r="D33" s="89" t="s">
+      <c r="D33" s="94" t="s">
         <v>42</v>
       </c>
       <c r="E33" s="5" t="s">
@@ -2852,9 +2858,9 @@
       <c r="T33" s="5"/>
     </row>
     <row r="34" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="85"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="90"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="95"/>
       <c r="E34" s="10" t="s">
         <v>1</v>
       </c>
@@ -2875,11 +2881,11 @@
       <c r="T34" s="10"/>
     </row>
     <row r="35" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="85"/>
-      <c r="C35" s="87">
+      <c r="B35" s="102"/>
+      <c r="C35" s="90">
         <v>15</v>
       </c>
-      <c r="D35" s="89" t="s">
+      <c r="D35" s="94" t="s">
         <v>44</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -2902,9 +2908,9 @@
       <c r="T35" s="5"/>
     </row>
     <row r="36" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="85"/>
-      <c r="C36" s="88"/>
-      <c r="D36" s="90"/>
+      <c r="B36" s="102"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="95"/>
       <c r="E36" s="10" t="s">
         <v>1</v>
       </c>
@@ -2925,11 +2931,11 @@
       <c r="T36" s="10"/>
     </row>
     <row r="37" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="85"/>
-      <c r="C37" s="87">
+      <c r="B37" s="102"/>
+      <c r="C37" s="90">
         <v>16</v>
       </c>
-      <c r="D37" s="89" t="s">
+      <c r="D37" s="94" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -2952,9 +2958,9 @@
       <c r="T37" s="27"/>
     </row>
     <row r="38" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="86"/>
-      <c r="C38" s="88"/>
-      <c r="D38" s="90"/>
+      <c r="B38" s="103"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="95"/>
       <c r="E38" s="10" t="s">
         <v>1</v>
       </c>
@@ -2975,13 +2981,13 @@
       <c r="T38" s="10"/>
     </row>
     <row r="39" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="84" t="s">
+      <c r="B39" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="87">
+      <c r="C39" s="90">
         <v>17</v>
       </c>
-      <c r="D39" s="89" t="s">
+      <c r="D39" s="94" t="s">
         <v>47</v>
       </c>
       <c r="E39" s="5" t="s">
@@ -3004,9 +3010,9 @@
       <c r="T39" s="7"/>
     </row>
     <row r="40" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="85"/>
-      <c r="C40" s="88"/>
-      <c r="D40" s="90"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="91"/>
+      <c r="D40" s="95"/>
       <c r="E40" s="10" t="s">
         <v>1</v>
       </c>
@@ -3027,11 +3033,11 @@
       <c r="T40" s="10"/>
     </row>
     <row r="41" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="85"/>
-      <c r="C41" s="87">
+      <c r="B41" s="102"/>
+      <c r="C41" s="90">
         <v>18</v>
       </c>
-      <c r="D41" s="89" t="s">
+      <c r="D41" s="94" t="s">
         <v>48</v>
       </c>
       <c r="E41" s="5" t="s">
@@ -3054,9 +3060,9 @@
       <c r="T41" s="7"/>
     </row>
     <row r="42" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="85"/>
-      <c r="C42" s="88"/>
-      <c r="D42" s="90"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="95"/>
       <c r="E42" s="10" t="s">
         <v>1</v>
       </c>
@@ -3077,11 +3083,11 @@
       <c r="T42" s="10"/>
     </row>
     <row r="43" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="85"/>
-      <c r="C43" s="87">
+      <c r="B43" s="102"/>
+      <c r="C43" s="90">
         <v>19</v>
       </c>
-      <c r="D43" s="89" t="s">
+      <c r="D43" s="94" t="s">
         <v>49</v>
       </c>
       <c r="E43" s="5" t="s">
@@ -3104,9 +3110,9 @@
       <c r="T43" s="7"/>
     </row>
     <row r="44" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="86"/>
-      <c r="C44" s="88"/>
-      <c r="D44" s="90"/>
+      <c r="B44" s="103"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="95"/>
       <c r="E44" s="10" t="s">
         <v>1</v>
       </c>
@@ -3127,13 +3133,13 @@
       <c r="T44" s="10"/>
     </row>
     <row r="45" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="84" t="s">
+      <c r="B45" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="87">
+      <c r="C45" s="90">
         <v>20</v>
       </c>
-      <c r="D45" s="89" t="s">
+      <c r="D45" s="94" t="s">
         <v>51</v>
       </c>
       <c r="E45" s="5" t="s">
@@ -3156,9 +3162,9 @@
       <c r="T45" s="35"/>
     </row>
     <row r="46" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="85"/>
-      <c r="C46" s="88"/>
-      <c r="D46" s="90"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="91"/>
+      <c r="D46" s="95"/>
       <c r="E46" s="10" t="s">
         <v>1</v>
       </c>
@@ -3179,11 +3185,11 @@
       <c r="T46" s="71"/>
     </row>
     <row r="47" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="85"/>
-      <c r="C47" s="87">
+      <c r="B47" s="102"/>
+      <c r="C47" s="90">
         <v>21</v>
       </c>
-      <c r="D47" s="89" t="s">
+      <c r="D47" s="94" t="s">
         <v>52</v>
       </c>
       <c r="E47" s="5" t="s">
@@ -3206,9 +3212,9 @@
       <c r="T47" s="7"/>
     </row>
     <row r="48" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="85"/>
-      <c r="C48" s="88"/>
-      <c r="D48" s="90"/>
+      <c r="B48" s="102"/>
+      <c r="C48" s="91"/>
+      <c r="D48" s="95"/>
       <c r="E48" s="10" t="s">
         <v>1</v>
       </c>
@@ -3229,11 +3235,11 @@
       <c r="T48" s="71"/>
     </row>
     <row r="49" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="85"/>
-      <c r="C49" s="87">
+      <c r="B49" s="102"/>
+      <c r="C49" s="90">
         <v>22</v>
       </c>
-      <c r="D49" s="89" t="s">
+      <c r="D49" s="94" t="s">
         <v>53</v>
       </c>
       <c r="E49" s="5" t="s">
@@ -3257,9 +3263,9 @@
       <c r="U49" s="43"/>
     </row>
     <row r="50" spans="2:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="86"/>
-      <c r="C50" s="88"/>
-      <c r="D50" s="90"/>
+      <c r="B50" s="103"/>
+      <c r="C50" s="91"/>
+      <c r="D50" s="95"/>
       <c r="E50" s="10" t="s">
         <v>1</v>
       </c>
@@ -3322,11 +3328,11 @@
       <c r="T52" s="83"/>
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B53" s="107" t="s">
+      <c r="B53" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="107"/>
-      <c r="D53" s="107"/>
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
       <c r="E53" s="83"/>
       <c r="F53" s="83"/>
       <c r="G53" s="83"/>
@@ -3345,10 +3351,10 @@
       <c r="T53" s="83"/>
     </row>
     <row r="54" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B54" s="107" t="s">
+      <c r="B54" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="107"/>
+      <c r="C54" s="87"/>
       <c r="D54" s="1" t="s">
         <v>19</v>
       </c>
@@ -3370,8 +3376,8 @@
       <c r="T54" s="83"/>
     </row>
     <row r="55" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B55" s="108"/>
-      <c r="C55" s="108"/>
+      <c r="B55" s="88"/>
+      <c r="C55" s="88"/>
       <c r="D55" s="1" t="s">
         <v>20</v>
       </c>
@@ -3393,8 +3399,8 @@
       <c r="T55" s="83"/>
     </row>
     <row r="56" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B56" s="109"/>
-      <c r="C56" s="109"/>
+      <c r="B56" s="89"/>
+      <c r="C56" s="89"/>
       <c r="D56" s="1" t="s">
         <v>21</v>
       </c>
@@ -3416,8 +3422,8 @@
       <c r="T56" s="83"/>
     </row>
     <row r="57" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B57" s="97"/>
-      <c r="C57" s="97"/>
+      <c r="B57" s="96"/>
+      <c r="C57" s="96"/>
       <c r="D57" s="1" t="s">
         <v>22</v>
       </c>
@@ -3440,6 +3446,57 @@
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B27:B38"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="B15:B24"/>
     <mergeCell ref="B6:T6"/>
     <mergeCell ref="B53:D53"/>
     <mergeCell ref="B54:C54"/>
@@ -3456,57 +3513,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="B15:B24"/>
-    <mergeCell ref="B27:B38"/>
-    <mergeCell ref="B39:B44"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B3:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>